<commit_message>
Corrige error en FCS_troceador
</commit_message>
<xml_diff>
--- a/variables anaFCS.xlsx
+++ b/variables anaFCS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>TACgain</t>
   </si>
@@ -46,6 +46,69 @@
   </si>
   <si>
     <t>FCSdata</t>
+  </si>
+  <si>
+    <t>FCSintervalos</t>
+  </si>
+  <si>
+    <t>FCSmean</t>
+  </si>
+  <si>
+    <t>Gintervalos</t>
+  </si>
+  <si>
+    <t>Gmean</t>
+  </si>
+  <si>
+    <t>acqTime</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>binFreq</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+  <si>
+    <t>intervalosPromediados</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>numIntervalos</t>
+  </si>
+  <si>
+    <t>numPuntosSeccion</t>
+  </si>
+  <si>
+    <t>Secciones</t>
+  </si>
+  <si>
+    <t>numSubIntervalosError</t>
+  </si>
+  <si>
+    <t>tData</t>
+  </si>
+  <si>
+    <t>tauLagMax</t>
+  </si>
+  <si>
+    <t>tipoCorrelacion</t>
+  </si>
+  <si>
+    <t>1,2, o 3 (cc)</t>
+  </si>
+  <si>
+    <t>auto o cross</t>
+  </si>
+  <si>
+    <t>Si es cross, hace todas</t>
+  </si>
+  <si>
+    <t>tiempo de los datos de FCSintervalos</t>
   </si>
 </sst>
 </file>
@@ -384,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:C12"/>
+  <dimension ref="A4:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,6 +501,106 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incluyo el promediado y la revisión de intervalos indiividuales
</commit_message>
<xml_diff>
--- a/variables anaFCS.xlsx
+++ b/variables anaFCS.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="17715" windowHeight="9030" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Variables ana_FCS" sheetId="1" r:id="rId1"/>
+    <sheet name="Variables raw files" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,14 +16,152 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+  <si>
+    <t xml:space="preserve">  FCSTraza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gintervalos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gintervalos_noAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gmean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gmean_noAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  acqTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  alfa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  alfaCoeff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  binFreq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  correctAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  cps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  cpsIntervalos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  fname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  h_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  intervalosPromediados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  isScanning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  numChannelsAcquisition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  numFiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  numIntervalos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  numPuntosSeccion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  numSecciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  numSubIntervalosError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  tTraza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  tauLagMax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  tau_AP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  tipoCorrelacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noAP </t>
+  </si>
+  <si>
+    <t>sn corregir el After Pulsing</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>True si corrige el afterpulsing</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Los números de los intervalos que se promedian</t>
+  </si>
+  <si>
+    <t>Tiempo correspondiente a tTraza</t>
+  </si>
+  <si>
+    <t>Trazas de adquisición para cada intervalo con binning de 0.01s para poder representarlas con facilidad</t>
+  </si>
+  <si>
+    <t>Dimensiones</t>
+  </si>
+  <si>
+    <t>uint16</t>
+  </si>
+  <si>
+    <t>Puntos X canales X intervalos</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>isScanning</t>
+  </si>
+  <si>
+    <t>photonArrivalTimes</t>
+  </si>
+  <si>
+    <t>TACrange</t>
+  </si>
   <si>
     <t>TACgain</t>
   </si>
   <si>
-    <t>TACrange</t>
-  </si>
-  <si>
     <t>imgDecode</t>
   </si>
   <si>
@@ -34,89 +172,22 @@
   </si>
   <si>
     <t>pixelSync</t>
-  </si>
-  <si>
-    <t>photonArrivalTimes</t>
-  </si>
-  <si>
-    <t>isScanning</t>
-  </si>
-  <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>FCSdata</t>
-  </si>
-  <si>
-    <t>FCSintervalos</t>
-  </si>
-  <si>
-    <t>FCSmean</t>
-  </si>
-  <si>
-    <t>Gintervalos</t>
-  </si>
-  <si>
-    <t>Gmean</t>
-  </si>
-  <si>
-    <t>acqTime</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>binFreq</t>
-  </si>
-  <si>
-    <t>channel</t>
-  </si>
-  <si>
-    <t>intervalosPromediados</t>
-  </si>
-  <si>
-    <t>logical</t>
-  </si>
-  <si>
-    <t>numIntervalos</t>
-  </si>
-  <si>
-    <t>numPuntosSeccion</t>
-  </si>
-  <si>
-    <t>Secciones</t>
-  </si>
-  <si>
-    <t>numSubIntervalosError</t>
-  </si>
-  <si>
-    <t>tData</t>
-  </si>
-  <si>
-    <t>tauLagMax</t>
-  </si>
-  <si>
-    <t>tipoCorrelacion</t>
-  </si>
-  <si>
-    <t>1,2, o 3 (cc)</t>
-  </si>
-  <si>
-    <t>auto o cross</t>
-  </si>
-  <si>
-    <t>Si es cross, hace todas</t>
-  </si>
-  <si>
-    <t>tiempo de los datos de FCSintervalos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,8 +215,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,175 +520,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>42206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="C30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>